<commit_message>
Forms updated with Rwanda and Kenya Regions and Education SYstems
</commit_message>
<xml_diff>
--- a/soil/soil_sample/soils.13.02.2015/VS_Eplot_soils_sample_02_07.2015_v1.xls.xlsx
+++ b/soil/soil_sample/soils.13.02.2015/VS_Eplot_soils_sample_02_07.2015_v1.xls.xlsx
@@ -13,57 +13,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="172">
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
   <si>
     <t>list name</t>
   </si>
   <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>label</t>
   </si>
   <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
+    <t>bind:relevant</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
+    <t>bind:constraint</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>constraint_message</t>
+  </si>
+  <si>
     <t>country</t>
   </si>
   <si>
     <t>TZA</t>
   </si>
   <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>choice_filter</t>
-  </si>
-  <si>
-    <t>bind:relevant</t>
-  </si>
-  <si>
-    <t>bind:constraint</t>
-  </si>
-  <si>
-    <t>appearance</t>
+    <t>start</t>
   </si>
   <si>
     <t>Tanzania</t>
   </si>
   <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>constraint_message</t>
+    <t>end</t>
   </si>
   <si>
     <t>GHA</t>
@@ -72,7 +81,7 @@
     <t>Ghana</t>
   </si>
   <si>
-    <t>start</t>
+    <t>today</t>
   </si>
   <si>
     <t>UGA</t>
@@ -81,36 +90,120 @@
     <t>Uganda</t>
   </si>
   <si>
-    <t>end</t>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>KEN</t>
+  </si>
+  <si>
+    <t>metadata</t>
+  </si>
+  <si>
+    <t>default_language</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>soils_eplot_sample_02_jul_2015_v1</t>
+  </si>
+  <si>
+    <t>select one from country</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>VS E-plot soils survey – 02 July 2015 v1</t>
+  </si>
+  <si>
+    <t>landscape_no</t>
+  </si>
+  <si>
+    <t>Landscape No</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>3 characters e.g L09. Enter 000 if N/A</t>
+  </si>
+  <si>
+    <t>string-length(.)=3</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>RWA</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
   </si>
   <si>
     <t>texture</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
     <t>sand</t>
   </si>
   <si>
-    <t>today</t>
-  </si>
-  <si>
-    <t>form_title</t>
-  </si>
-  <si>
-    <t>begin group</t>
-  </si>
-  <si>
-    <t>metadata</t>
+    <t>eplot_no</t>
+  </si>
+  <si>
+    <t>Eplot No</t>
+  </si>
+  <si>
+    <t>Sequential number from 000 - 999</t>
+  </si>
+  <si>
+    <t>regex(., '^\d\d\d$')</t>
+  </si>
+  <si>
+    <t>numbers</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>eplot_code</t>
+  </si>
+  <si>
+    <t>concat(${country}, '-', ${landscape_no}, '-', ${eplot_no})</t>
+  </si>
+  <si>
+    <t>name_group</t>
+  </si>
+  <si>
+    <t>field-list</t>
   </si>
   <si>
     <t>Sand</t>
   </si>
   <si>
+    <t>sampler_first_name</t>
+  </si>
+  <si>
     <t>loam</t>
   </si>
   <si>
+    <t>First Name of person sampling and weighing samples</t>
+  </si>
+  <si>
     <t>Loam</t>
   </si>
   <si>
+    <t>First Name</t>
+  </si>
+  <si>
     <t>loamy_sand</t>
   </si>
   <si>
@@ -132,16 +225,10 @@
     <t>sandy_clay_loam</t>
   </si>
   <si>
-    <t>select one from country</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>text</t>
+    <t>sampler_last_name</t>
+  </si>
+  <si>
+    <t>Last Name of person sampling and weighing samples</t>
   </si>
   <si>
     <t>Sandy Clay Loam</t>
@@ -165,6 +252,9 @@
     <t>Sandy Clay</t>
   </si>
   <si>
+    <t>Last Name</t>
+  </si>
+  <si>
     <t>clay</t>
   </si>
   <si>
@@ -175,84 +265,6 @@
   </si>
   <si>
     <t>Silty Clay</t>
-  </si>
-  <si>
-    <t>default_language</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>soils_eplot_sample_02_jul_2015_v1</t>
-  </si>
-  <si>
-    <t>VS E-plot soils survey – 02 July 2015 v1</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>landscape_no</t>
-  </si>
-  <si>
-    <t>Landscape No</t>
-  </si>
-  <si>
-    <t>3 characters e.g L09. Enter 000 if N/A</t>
-  </si>
-  <si>
-    <t>string-length(.)=3</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>eplot_no</t>
-  </si>
-  <si>
-    <t>Eplot No</t>
-  </si>
-  <si>
-    <t>Sequential number from 000 - 999</t>
-  </si>
-  <si>
-    <t>regex(., '^\d\d\d$')</t>
-  </si>
-  <si>
-    <t>numbers</t>
-  </si>
-  <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>eplot_code</t>
-  </si>
-  <si>
-    <t>concat(${country}, '-', ${landscape_no}, '-', ${eplot_no})</t>
-  </si>
-  <si>
-    <t>name_group</t>
-  </si>
-  <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>sampler_first_name</t>
-  </si>
-  <si>
-    <t>First Name of person sampling and weighing samples</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>sampler_last_name</t>
-  </si>
-  <si>
-    <t>Last Name of person sampling and weighing samples</t>
-  </si>
-  <si>
-    <t>Last Name</t>
   </si>
   <si>
     <t>date</t>
@@ -523,7 +535,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -535,13 +547,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10.0"/>
       <color rgb="FF333333"/>
       <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="9.0"/>
@@ -554,6 +566,9 @@
     </font>
     <font>
       <sz val="8.0"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -585,6 +600,20 @@
       <bottom/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3C3C3C"/>
       </left>
@@ -598,49 +627,31 @@
         <color rgb="FF3C3C3C"/>
       </bottom>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFC0C0C0"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFC0C0C0"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFC0C0C0"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFC0C0C0"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="1" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -648,11 +659,17 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="1" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -691,16 +708,16 @@
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>55</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -714,16 +731,16 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="A2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4">
         <v>1.0</v>
       </c>
       <c r="E2" s="2"/>
@@ -1045,7 +1062,7 @@
   <sheetData>
     <row r="1" ht="11.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1081,13 +1098,13 @@
     </row>
     <row r="3" ht="11.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1102,13 +1119,13 @@
     </row>
     <row r="4" ht="11.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1123,13 +1140,13 @@
     </row>
     <row r="5" ht="11.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1143,9 +1160,15 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" ht="11.25" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1158,9 +1181,15 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" ht="11.25" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1173,15 +1202,9 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" ht="11.25" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1194,15 +1217,9 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" ht="11.25" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1215,15 +1232,9 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" ht="11.25" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1237,13 +1248,13 @@
     </row>
     <row r="11" ht="11.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1258,13 +1269,13 @@
     </row>
     <row r="12" ht="11.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1279,13 +1290,13 @@
     </row>
     <row r="13" ht="11.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1300,13 +1311,13 @@
     </row>
     <row r="14" ht="11.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>45</v>
+      <c r="B14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1321,13 +1332,13 @@
     </row>
     <row r="15" ht="11.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1342,13 +1353,13 @@
     </row>
     <row r="16" ht="11.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1363,13 +1374,13 @@
     </row>
     <row r="17" ht="11.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1384,13 +1395,13 @@
     </row>
     <row r="18" ht="11.25" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1404,9 +1415,15 @@
       <c r="M18" s="2"/>
     </row>
     <row r="19" ht="11.25" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1419,9 +1436,15 @@
       <c r="M19" s="2"/>
     </row>
     <row r="20" ht="11.25" customHeight="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>81</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1434,9 +1457,15 @@
       <c r="M20" s="2"/>
     </row>
     <row r="21" ht="11.25" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -3803,7 +3832,7 @@
       <c r="L178" s="2"/>
       <c r="M178" s="2"/>
     </row>
-    <row r="179" ht="13.5" customHeight="1">
+    <row r="179" ht="11.25" customHeight="1">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3817,6 +3846,51 @@
       <c r="K179" s="2"/>
       <c r="L179" s="2"/>
       <c r="M179" s="2"/>
+    </row>
+    <row r="180" ht="11.25" customHeight="1">
+      <c r="A180" s="2"/>
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2"/>
+      <c r="F180" s="2"/>
+      <c r="G180" s="2"/>
+      <c r="H180" s="2"/>
+      <c r="I180" s="2"/>
+      <c r="J180" s="2"/>
+      <c r="K180" s="2"/>
+      <c r="L180" s="2"/>
+      <c r="M180" s="2"/>
+    </row>
+    <row r="181" ht="11.25" customHeight="1">
+      <c r="A181" s="2"/>
+      <c r="B181" s="2"/>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
+      <c r="G181" s="2"/>
+      <c r="H181" s="2"/>
+      <c r="I181" s="2"/>
+      <c r="J181" s="2"/>
+      <c r="K181" s="2"/>
+      <c r="L181" s="2"/>
+      <c r="M181" s="2"/>
+    </row>
+    <row r="182" ht="13.5" customHeight="1">
+      <c r="A182" s="2"/>
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
+      <c r="G182" s="2"/>
+      <c r="H182" s="2"/>
+      <c r="I182" s="2"/>
+      <c r="J182" s="2"/>
+      <c r="K182" s="2"/>
+      <c r="L182" s="2"/>
+      <c r="M182" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3848,7 +3922,7 @@
   <sheetData>
     <row r="1" ht="11.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -3857,31 +3931,31 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -3896,10 +3970,10 @@
     </row>
     <row r="2" ht="11.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3924,10 +3998,10 @@
     </row>
     <row r="3" ht="11.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3952,10 +4026,10 @@
     </row>
     <row r="4" ht="11.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3980,10 +4054,10 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -4008,13 +4082,13 @@
     </row>
     <row r="6" ht="11.25" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -4022,7 +4096,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -4039,26 +4113,26 @@
       <c r="V6" s="2"/>
     </row>
     <row r="7" ht="11.25" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="13"/>
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="12"/>
       <c r="I7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="J7" s="12"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -4072,28 +4146,28 @@
       <c r="V7" s="2"/>
     </row>
     <row r="8" ht="11.25" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>68</v>
+      <c r="A8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="J8" s="12"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -4107,21 +4181,21 @@
       <c r="V8" s="2"/>
     </row>
     <row r="9" ht="11.25" customHeight="1">
-      <c r="A9" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="10" t="s">
-        <v>71</v>
+      <c r="A9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -4137,10 +4211,10 @@
     </row>
     <row r="10" ht="11.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -4148,7 +4222,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -4167,23 +4241,23 @@
     </row>
     <row r="11" ht="11.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -4201,13 +4275,13 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>78</v>
+        <v>70</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>79</v>
@@ -4217,7 +4291,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -4234,22 +4308,22 @@
       <c r="V12" s="2"/>
     </row>
     <row r="13" ht="11.25" customHeight="1">
-      <c r="A13" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>82</v>
+      <c r="A13" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="15" t="s">
-        <v>41</v>
+      <c r="I13" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -4267,7 +4341,7 @@
     </row>
     <row r="14" ht="11.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4293,13 +4367,13 @@
     </row>
     <row r="15" ht="11.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -4307,7 +4381,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -4325,13 +4399,13 @@
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -4339,7 +4413,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -4357,7 +4431,7 @@
     </row>
     <row r="17" ht="11.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4383,10 +4457,10 @@
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -4394,7 +4468,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -4413,11 +4487,11 @@
     </row>
     <row r="19" ht="11.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -4441,28 +4515,28 @@
     </row>
     <row r="20" ht="12.0" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -4477,28 +4551,28 @@
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -4513,13 +4587,13 @@
     </row>
     <row r="22" ht="12.0" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -4527,7 +4601,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -4545,23 +4619,23 @@
     </row>
     <row r="23" ht="12.0" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -4579,23 +4653,23 @@
     </row>
     <row r="24" ht="12.0" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -4613,7 +4687,7 @@
     </row>
     <row r="25" ht="11.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4663,20 +4737,20 @@
     </row>
     <row r="27" ht="12.0" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -4695,11 +4769,11 @@
     </row>
     <row r="28" ht="11.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -4723,28 +4797,28 @@
     </row>
     <row r="29" ht="12.0" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="2"/>
       <c r="G29" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4759,28 +4833,28 @@
     </row>
     <row r="30" ht="12.0" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4795,13 +4869,13 @@
     </row>
     <row r="31" ht="12.0" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -4809,7 +4883,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -4827,23 +4901,23 @@
     </row>
     <row r="32" ht="12.0" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -4861,23 +4935,23 @@
     </row>
     <row r="33" ht="12.0" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -4895,7 +4969,7 @@
     </row>
     <row r="34" ht="11.25" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -4945,20 +5019,20 @@
     </row>
     <row r="36" ht="12.0" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -4977,11 +5051,11 @@
     </row>
     <row r="37" ht="11.25" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -5005,28 +5079,28 @@
     </row>
     <row r="38" ht="12.0" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="2"/>
       <c r="G38" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5041,28 +5115,28 @@
     </row>
     <row r="39" ht="12.0" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5077,13 +5151,13 @@
     </row>
     <row r="40" ht="12.0" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -5091,7 +5165,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -5109,23 +5183,23 @@
     </row>
     <row r="41" ht="12.0" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -5143,23 +5217,23 @@
     </row>
     <row r="42" ht="12.0" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -5177,13 +5251,13 @@
     </row>
     <row r="43" ht="12.0" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -5191,7 +5265,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -5209,7 +5283,7 @@
     </row>
     <row r="44" ht="11.25" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -5259,20 +5333,20 @@
     </row>
     <row r="46" ht="12.0" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -5291,11 +5365,11 @@
     </row>
     <row r="47" ht="11.25" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -5319,28 +5393,28 @@
     </row>
     <row r="48" ht="12.0" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="2"/>
       <c r="G48" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="15" t="s">
-        <v>136</v>
+      <c r="L48" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -5355,28 +5429,28 @@
     </row>
     <row r="49" ht="12.0" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -5391,13 +5465,13 @@
     </row>
     <row r="50" ht="12.0" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -5405,7 +5479,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -5423,23 +5497,23 @@
     </row>
     <row r="51" ht="12.0" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -5457,23 +5531,23 @@
     </row>
     <row r="52" ht="12.0" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -5491,13 +5565,13 @@
     </row>
     <row r="53" ht="12.0" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -5505,7 +5579,7 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -5523,7 +5597,7 @@
     </row>
     <row r="54" ht="11.25" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -5573,10 +5647,10 @@
     </row>
     <row r="56" ht="12.0" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -5584,7 +5658,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -5603,11 +5677,11 @@
     </row>
     <row r="57" ht="11.25" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -5631,28 +5705,28 @@
     </row>
     <row r="58" ht="12.0" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -5667,7 +5741,7 @@
     </row>
     <row r="59" ht="11.25" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -5717,20 +5791,20 @@
     </row>
     <row r="61" ht="12.0" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -5749,11 +5823,11 @@
     </row>
     <row r="62" ht="11.25" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -5777,28 +5851,28 @@
     </row>
     <row r="63" ht="12.0" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -5813,7 +5887,7 @@
     </row>
     <row r="64" ht="11.25" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -5863,10 +5937,10 @@
     </row>
     <row r="66" ht="12.0" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -5874,7 +5948,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
@@ -5893,11 +5967,11 @@
     </row>
     <row r="67" ht="11.25" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -5921,28 +5995,28 @@
     </row>
     <row r="68" ht="12.0" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -5957,7 +6031,7 @@
     </row>
     <row r="69" ht="11.25" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -6007,20 +6081,20 @@
     </row>
     <row r="71" ht="12.0" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
@@ -6039,11 +6113,11 @@
     </row>
     <row r="72" ht="11.25" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -6067,28 +6141,28 @@
     </row>
     <row r="73" ht="12.0" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -6103,7 +6177,7 @@
     </row>
     <row r="74" ht="11.25" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -6153,10 +6227,10 @@
     </row>
     <row r="76" ht="12.0" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -6164,7 +6238,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -6183,11 +6257,11 @@
     </row>
     <row r="77" ht="11.25" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -6211,28 +6285,28 @@
     </row>
     <row r="78" ht="12.0" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -6247,7 +6321,7 @@
     </row>
     <row r="79" ht="11.25" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -6297,20 +6371,20 @@
     </row>
     <row r="81" ht="12.0" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -6329,11 +6403,11 @@
     </row>
     <row r="82" ht="12.0" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -6343,7 +6417,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -6358,21 +6432,21 @@
     </row>
     <row r="83" ht="12.0" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
@@ -6392,7 +6466,7 @@
     </row>
     <row r="84" ht="11.25" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -6418,7 +6492,7 @@
     </row>
     <row r="85" ht="12.0" customHeight="1">
       <c r="A85" s="1"/>
-      <c r="B85" s="15"/>
+      <c r="B85" s="17"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -6442,10 +6516,10 @@
     </row>
     <row r="86" ht="12.0" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B86" s="15" t="s">
-        <v>163</v>
+        <v>25</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -6453,7 +6527,7 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -6472,11 +6546,11 @@
     </row>
     <row r="87" ht="12.0" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B87" s="1"/>
-      <c r="C87" s="15" t="s">
-        <v>164</v>
+      <c r="C87" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -6487,7 +6561,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -6502,13 +6576,13 @@
     </row>
     <row r="88" ht="12.0" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B88" s="15" t="s">
-        <v>165</v>
+        <v>132</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -6516,7 +6590,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
@@ -6534,7 +6608,7 @@
     </row>
     <row r="89" ht="12.0" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -6584,10 +6658,10 @@
     </row>
     <row r="91" ht="12.0" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>166</v>
+        <v>25</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -6595,7 +6669,7 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
@@ -6614,11 +6688,11 @@
     </row>
     <row r="92" ht="12.0" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B92" s="1"/>
-      <c r="C92" s="15" t="s">
-        <v>167</v>
+      <c r="C92" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -6629,7 +6703,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
       <c r="L92" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -6644,13 +6718,13 @@
     </row>
     <row r="93" ht="12.0" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B93" s="15" t="s">
-        <v>165</v>
+        <v>132</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -6658,7 +6732,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
@@ -6676,7 +6750,7 @@
     </row>
     <row r="94" ht="12.0" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>

</xml_diff>